<commit_message>
Criação do arquivo ASTAH com Diagrama de Casos de Uso
</commit_message>
<xml_diff>
--- a/Projetos 2016-1.xlsx
+++ b/Projetos 2016-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gvs\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gvs\git\pescapreco\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,25 +74,25 @@
     <t>Alexandre Henrique</t>
   </si>
   <si>
-    <t>SupermercAll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foodiscount </t>
-  </si>
-  <si>
     <t>Emanoel Ronnyer</t>
   </si>
   <si>
     <t>Daniel Fontenele</t>
   </si>
   <si>
-    <t>Ponto Eletrônico</t>
-  </si>
-  <si>
     <t>Felipe Rodrigues</t>
   </si>
   <si>
     <t>Washington da Costa</t>
+  </si>
+  <si>
+    <t>Roga Multimarcas</t>
+  </si>
+  <si>
+    <t>eCortesia</t>
+  </si>
+  <si>
+    <t>Orologio Webponto</t>
   </si>
 </sst>
 </file>
@@ -154,8 +154,36 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -432,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +532,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -517,28 +545,28 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>